<commit_message>
Updating code + adata files.
</commit_message>
<xml_diff>
--- a/data/ecoli_interactions.xlsx
+++ b/data/ecoli_interactions.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\github\CARAMeL\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4CBB3B46-B991-4292-81C4-DFE8F1DFB3A6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{12BE2DFE-5DC3-4FF0-B04C-D2DB73719E7A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="22932" yWindow="-84" windowWidth="11016" windowHeight="17040" activeTab="1" xr2:uid="{ACD11B47-A1BF-4BB5-A276-4A778C038C67}"/>
   </bookViews>
@@ -62,7 +62,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5070" uniqueCount="227">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5190" uniqueCount="336">
   <si>
     <t>Code</t>
   </si>
@@ -739,10 +739,337 @@
     <t>CEFSULODIN-6.0,MCILLINAM-0.03</t>
   </si>
   <si>
-    <t>CRN</t>
+    <t>C90</t>
   </si>
   <si>
-    <t>C90</t>
+    <t>CRL</t>
+  </si>
+  <si>
+    <t>CPZ</t>
+  </si>
+  <si>
+    <t>CHO</t>
+  </si>
+  <si>
+    <t>CPT</t>
+  </si>
+  <si>
+    <t>CSD</t>
+  </si>
+  <si>
+    <t>DCH</t>
+  </si>
+  <si>
+    <t>CERULENIN-6.0</t>
+  </si>
+  <si>
+    <t>CHIR090-0.075</t>
+  </si>
+  <si>
+    <t>CHLOROPROMAZINE-24</t>
+  </si>
+  <si>
+    <t>CHOLATE-2.0%</t>
+  </si>
+  <si>
+    <t>CISPLATIN-100</t>
+  </si>
+  <si>
+    <t>CYCLOSERINED-16</t>
+  </si>
+  <si>
+    <t>DEOXYCHOLATE-2.0%</t>
+  </si>
+  <si>
+    <t>DBC</t>
+  </si>
+  <si>
+    <t>EDTA</t>
+  </si>
+  <si>
+    <t>EGCG</t>
+  </si>
+  <si>
+    <t>EGTA</t>
+  </si>
+  <si>
+    <t>EPI</t>
+  </si>
+  <si>
+    <t>ETH</t>
+  </si>
+  <si>
+    <t>DIBUCAINE-1.2</t>
+  </si>
+  <si>
+    <t>DXR</t>
+  </si>
+  <si>
+    <t>DOXORUBICIN-10.0</t>
+  </si>
+  <si>
+    <t>EDTA-1.0</t>
+  </si>
+  <si>
+    <t>EGCG-50</t>
+  </si>
+  <si>
+    <t>EGTA-2.0</t>
+  </si>
+  <si>
+    <t>EPINEPHRINE-1000</t>
+  </si>
+  <si>
+    <t>ETHANOL-6.0</t>
+  </si>
+  <si>
+    <t>EDB</t>
+  </si>
+  <si>
+    <t>ETHIDIUMBROMIDE-50</t>
+  </si>
+  <si>
+    <t>GLUCOSAMINE</t>
+  </si>
+  <si>
+    <t>GFOS</t>
+  </si>
+  <si>
+    <t>HUREA</t>
+  </si>
+  <si>
+    <t>INDO</t>
+  </si>
+  <si>
+    <t>LFE</t>
+  </si>
+  <si>
+    <t>HCO</t>
+  </si>
+  <si>
+    <t>HCU</t>
+  </si>
+  <si>
+    <t>HFE</t>
+  </si>
+  <si>
+    <t>HNI</t>
+  </si>
+  <si>
+    <t>INZ</t>
+  </si>
+  <si>
+    <t>MALTOSE</t>
+  </si>
+  <si>
+    <t>MEC</t>
+  </si>
+  <si>
+    <t>MTX</t>
+  </si>
+  <si>
+    <t>MMC</t>
+  </si>
+  <si>
+    <t>MMS</t>
+  </si>
+  <si>
+    <t>GLUFOSFOMYCIN-0.2</t>
+  </si>
+  <si>
+    <t>HIGHCOBALT-0.5</t>
+  </si>
+  <si>
+    <t>HIGHCOPPER-4.0</t>
+  </si>
+  <si>
+    <t>HIGHFE</t>
+  </si>
+  <si>
+    <t>HIGHNICKEL-1.0</t>
+  </si>
+  <si>
+    <t>HYDROXYUREA-10.0</t>
+  </si>
+  <si>
+    <t>INDOLICIDIN-0.1</t>
+  </si>
+  <si>
+    <t>ISONIAZID-1.5</t>
+  </si>
+  <si>
+    <t>LOWFE</t>
+  </si>
+  <si>
+    <t>MECILLINAM-0.12</t>
+  </si>
+  <si>
+    <t>METHOTREXATE-25</t>
+  </si>
+  <si>
+    <t>MITOMYCINC-0.1</t>
+  </si>
+  <si>
+    <t>MMS-0.05%</t>
+  </si>
+  <si>
+    <t>NAG</t>
+  </si>
+  <si>
+    <t>NACL</t>
+  </si>
+  <si>
+    <t>NH4CL</t>
+  </si>
+  <si>
+    <t>NIG</t>
+  </si>
+  <si>
+    <t>NEPI</t>
+  </si>
+  <si>
+    <t>NOV</t>
+  </si>
+  <si>
+    <t>PQ</t>
+  </si>
+  <si>
+    <t>N-ACETYLGLUCOSAMINE</t>
+  </si>
+  <si>
+    <t>NACL-600</t>
+  </si>
+  <si>
+    <t>NIGERICIN-5.0</t>
+  </si>
+  <si>
+    <t>NOREPINEPHRINE-1000</t>
+  </si>
+  <si>
+    <t>NOVOBIOCIN-30</t>
+  </si>
+  <si>
+    <t>PARAQUAT-18.0</t>
+  </si>
+  <si>
+    <t>PH4</t>
+  </si>
+  <si>
+    <t>PH10</t>
+  </si>
+  <si>
+    <t>PHL</t>
+  </si>
+  <si>
+    <t>PRO</t>
+  </si>
+  <si>
+    <t>PPI</t>
+  </si>
+  <si>
+    <t>PUR</t>
+  </si>
+  <si>
+    <t>PYO</t>
+  </si>
+  <si>
+    <t>RAD</t>
+  </si>
+  <si>
+    <t>PHLEOMYCIN-1.0</t>
+  </si>
+  <si>
+    <t>PMS</t>
+  </si>
+  <si>
+    <t>PMS-0.1</t>
+  </si>
+  <si>
+    <t>PROCAINE-30</t>
+  </si>
+  <si>
+    <t>PROPIDIUMIODIDE-50</t>
+  </si>
+  <si>
+    <t>PUROMYCIN-25</t>
+  </si>
+  <si>
+    <t>PYOCYANIN-10.0</t>
+  </si>
+  <si>
+    <t>RADICICOL-10</t>
+  </si>
+  <si>
+    <t>SDS</t>
+  </si>
+  <si>
+    <t>SDSEDTA</t>
+  </si>
+  <si>
+    <t>STN</t>
+  </si>
+  <si>
+    <t>SUCCINATE</t>
+  </si>
+  <si>
+    <t>SMZ</t>
+  </si>
+  <si>
+    <t>TCHO</t>
+  </si>
+  <si>
+    <t>THP</t>
+  </si>
+  <si>
+    <t>TLM</t>
+  </si>
+  <si>
+    <t>SDS-4.0%</t>
+  </si>
+  <si>
+    <t>SDS1.0%/EDTA0.5</t>
+  </si>
+  <si>
+    <t>SULFAMETHIZOLE-300</t>
+  </si>
+  <si>
+    <t>TAUROCHOLATE-1.0%</t>
+  </si>
+  <si>
+    <t>THEOPHYLLINE-100</t>
+  </si>
+  <si>
+    <t>THIOLACTOMYCIN-50</t>
+  </si>
+  <si>
+    <t>TMPSMZ</t>
+  </si>
+  <si>
+    <t>TTX</t>
+  </si>
+  <si>
+    <t>TUN</t>
+  </si>
+  <si>
+    <t>UV</t>
+  </si>
+  <si>
+    <t>VERA</t>
+  </si>
+  <si>
+    <t>TRIMETHOPRIM-0.1,SULFAMETHIZOLE-50</t>
+  </si>
+  <si>
+    <t>TRITONX-0.2%</t>
+  </si>
+  <si>
+    <t>TUNICAMYCIN-7.5</t>
+  </si>
+  <si>
+    <t>UV-24SEC</t>
+  </si>
+  <si>
+    <t>VERAPAMIL-1.0</t>
   </si>
 </sst>
 </file>
@@ -1425,11 +1752,11 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{248540B4-05A5-41ED-B00E-205943209F06}">
-  <dimension ref="A1:B56"/>
+  <dimension ref="A1:B115"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A23" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A57" sqref="A57"/>
+      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="B115" sqref="B115"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1872,12 +2199,490 @@
     </row>
     <row r="55" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A55" t="s">
-        <v>225</v>
+        <v>226</v>
+      </c>
+      <c r="B55" t="s">
+        <v>232</v>
       </c>
     </row>
     <row r="56" spans="1:2" x14ac:dyDescent="0.3">
       <c r="A56" t="s">
-        <v>226</v>
+        <v>225</v>
+      </c>
+      <c r="B56" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="57" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A57" t="s">
+        <v>227</v>
+      </c>
+      <c r="B57" t="s">
+        <v>234</v>
+      </c>
+    </row>
+    <row r="58" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A58" t="s">
+        <v>228</v>
+      </c>
+      <c r="B58" t="s">
+        <v>235</v>
+      </c>
+    </row>
+    <row r="59" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A59" t="s">
+        <v>229</v>
+      </c>
+      <c r="B59" t="s">
+        <v>236</v>
+      </c>
+    </row>
+    <row r="60" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A60" t="s">
+        <v>230</v>
+      </c>
+      <c r="B60" t="s">
+        <v>237</v>
+      </c>
+    </row>
+    <row r="61" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A61" t="s">
+        <v>231</v>
+      </c>
+      <c r="B61" t="s">
+        <v>238</v>
+      </c>
+    </row>
+    <row r="62" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A62" t="s">
+        <v>239</v>
+      </c>
+      <c r="B62" t="s">
+        <v>245</v>
+      </c>
+    </row>
+    <row r="63" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A63" t="s">
+        <v>246</v>
+      </c>
+      <c r="B63" t="s">
+        <v>247</v>
+      </c>
+    </row>
+    <row r="64" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A64" t="s">
+        <v>240</v>
+      </c>
+      <c r="B64" t="s">
+        <v>248</v>
+      </c>
+    </row>
+    <row r="65" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A65" t="s">
+        <v>241</v>
+      </c>
+      <c r="B65" t="s">
+        <v>249</v>
+      </c>
+    </row>
+    <row r="66" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A66" t="s">
+        <v>242</v>
+      </c>
+      <c r="B66" t="s">
+        <v>250</v>
+      </c>
+    </row>
+    <row r="67" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A67" t="s">
+        <v>243</v>
+      </c>
+      <c r="B67" t="s">
+        <v>251</v>
+      </c>
+    </row>
+    <row r="68" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A68" t="s">
+        <v>244</v>
+      </c>
+      <c r="B68" t="s">
+        <v>252</v>
+      </c>
+    </row>
+    <row r="69" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A69" t="s">
+        <v>253</v>
+      </c>
+      <c r="B69" t="s">
+        <v>254</v>
+      </c>
+    </row>
+    <row r="70" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A70" t="s">
+        <v>255</v>
+      </c>
+      <c r="B70" t="s">
+        <v>255</v>
+      </c>
+    </row>
+    <row r="71" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A71" t="s">
+        <v>183</v>
+      </c>
+      <c r="B71" t="s">
+        <v>183</v>
+      </c>
+    </row>
+    <row r="72" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A72" t="s">
+        <v>256</v>
+      </c>
+      <c r="B72" t="s">
+        <v>270</v>
+      </c>
+    </row>
+    <row r="73" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A73" t="s">
+        <v>184</v>
+      </c>
+      <c r="B73" t="s">
+        <v>184</v>
+      </c>
+    </row>
+    <row r="74" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A74" t="s">
+        <v>260</v>
+      </c>
+      <c r="B74" t="s">
+        <v>271</v>
+      </c>
+    </row>
+    <row r="75" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A75" t="s">
+        <v>261</v>
+      </c>
+      <c r="B75" t="s">
+        <v>272</v>
+      </c>
+    </row>
+    <row r="76" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A76" t="s">
+        <v>262</v>
+      </c>
+      <c r="B76" t="s">
+        <v>273</v>
+      </c>
+    </row>
+    <row r="77" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A77" t="s">
+        <v>263</v>
+      </c>
+      <c r="B77" t="s">
+        <v>274</v>
+      </c>
+    </row>
+    <row r="78" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A78" t="s">
+        <v>257</v>
+      </c>
+      <c r="B78" t="s">
+        <v>275</v>
+      </c>
+    </row>
+    <row r="79" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A79" t="s">
+        <v>258</v>
+      </c>
+      <c r="B79" t="s">
+        <v>276</v>
+      </c>
+    </row>
+    <row r="80" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A80" t="s">
+        <v>264</v>
+      </c>
+      <c r="B80" t="s">
+        <v>277</v>
+      </c>
+    </row>
+    <row r="81" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A81" t="s">
+        <v>259</v>
+      </c>
+      <c r="B81" t="s">
+        <v>278</v>
+      </c>
+    </row>
+    <row r="82" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A82" t="s">
+        <v>265</v>
+      </c>
+      <c r="B82" t="s">
+        <v>265</v>
+      </c>
+    </row>
+    <row r="83" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A83" t="s">
+        <v>266</v>
+      </c>
+      <c r="B83" t="s">
+        <v>279</v>
+      </c>
+    </row>
+    <row r="84" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A84" t="s">
+        <v>267</v>
+      </c>
+      <c r="B84" t="s">
+        <v>280</v>
+      </c>
+    </row>
+    <row r="85" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A85" t="s">
+        <v>268</v>
+      </c>
+      <c r="B85" t="s">
+        <v>281</v>
+      </c>
+    </row>
+    <row r="86" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A86" t="s">
+        <v>269</v>
+      </c>
+      <c r="B86" t="s">
+        <v>282</v>
+      </c>
+    </row>
+    <row r="87" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A87" t="s">
+        <v>283</v>
+      </c>
+      <c r="B87" t="s">
+        <v>290</v>
+      </c>
+    </row>
+    <row r="88" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A88" t="s">
+        <v>284</v>
+      </c>
+      <c r="B88" t="s">
+        <v>291</v>
+      </c>
+    </row>
+    <row r="89" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A89" t="s">
+        <v>285</v>
+      </c>
+      <c r="B89" t="s">
+        <v>285</v>
+      </c>
+    </row>
+    <row r="90" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A90" t="s">
+        <v>286</v>
+      </c>
+      <c r="B90" t="s">
+        <v>292</v>
+      </c>
+    </row>
+    <row r="91" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A91" t="s">
+        <v>287</v>
+      </c>
+      <c r="B91" t="s">
+        <v>293</v>
+      </c>
+    </row>
+    <row r="92" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A92" t="s">
+        <v>288</v>
+      </c>
+      <c r="B92" t="s">
+        <v>294</v>
+      </c>
+    </row>
+    <row r="93" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A93" t="s">
+        <v>289</v>
+      </c>
+      <c r="B93" t="s">
+        <v>295</v>
+      </c>
+    </row>
+    <row r="94" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A94" t="s">
+        <v>296</v>
+      </c>
+      <c r="B94" t="s">
+        <v>296</v>
+      </c>
+    </row>
+    <row r="95" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A95" t="s">
+        <v>297</v>
+      </c>
+      <c r="B95" t="s">
+        <v>297</v>
+      </c>
+    </row>
+    <row r="96" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A96" t="s">
+        <v>298</v>
+      </c>
+      <c r="B96" t="s">
+        <v>304</v>
+      </c>
+    </row>
+    <row r="97" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A97" t="s">
+        <v>305</v>
+      </c>
+      <c r="B97" t="s">
+        <v>306</v>
+      </c>
+    </row>
+    <row r="98" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A98" t="s">
+        <v>299</v>
+      </c>
+      <c r="B98" t="s">
+        <v>307</v>
+      </c>
+    </row>
+    <row r="99" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A99" t="s">
+        <v>300</v>
+      </c>
+      <c r="B99" t="s">
+        <v>308</v>
+      </c>
+    </row>
+    <row r="100" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A100" t="s">
+        <v>301</v>
+      </c>
+      <c r="B100" t="s">
+        <v>309</v>
+      </c>
+    </row>
+    <row r="101" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A101" t="s">
+        <v>302</v>
+      </c>
+      <c r="B101" t="s">
+        <v>310</v>
+      </c>
+    </row>
+    <row r="102" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A102" t="s">
+        <v>303</v>
+      </c>
+      <c r="B102" t="s">
+        <v>311</v>
+      </c>
+    </row>
+    <row r="103" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A103" t="s">
+        <v>312</v>
+      </c>
+      <c r="B103" t="s">
+        <v>320</v>
+      </c>
+    </row>
+    <row r="104" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A104" t="s">
+        <v>313</v>
+      </c>
+      <c r="B104" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="105" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A105" t="s">
+        <v>314</v>
+      </c>
+      <c r="B105" t="s">
+        <v>321</v>
+      </c>
+    </row>
+    <row r="106" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A106" t="s">
+        <v>315</v>
+      </c>
+      <c r="B106" t="s">
+        <v>315</v>
+      </c>
+    </row>
+    <row r="107" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A107" t="s">
+        <v>316</v>
+      </c>
+      <c r="B107" t="s">
+        <v>322</v>
+      </c>
+    </row>
+    <row r="108" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A108" t="s">
+        <v>317</v>
+      </c>
+      <c r="B108" t="s">
+        <v>323</v>
+      </c>
+    </row>
+    <row r="109" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A109" t="s">
+        <v>318</v>
+      </c>
+      <c r="B109" t="s">
+        <v>324</v>
+      </c>
+    </row>
+    <row r="110" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A110" t="s">
+        <v>319</v>
+      </c>
+      <c r="B110" t="s">
+        <v>325</v>
+      </c>
+    </row>
+    <row r="111" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A111" t="s">
+        <v>326</v>
+      </c>
+      <c r="B111" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="112" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A112" t="s">
+        <v>327</v>
+      </c>
+      <c r="B112" t="s">
+        <v>332</v>
+      </c>
+    </row>
+    <row r="113" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A113" t="s">
+        <v>328</v>
+      </c>
+      <c r="B113" t="s">
+        <v>333</v>
+      </c>
+    </row>
+    <row r="114" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A114" t="s">
+        <v>329</v>
+      </c>
+      <c r="B114" t="s">
+        <v>334</v>
+      </c>
+    </row>
+    <row r="115" spans="1:2" x14ac:dyDescent="0.3">
+      <c r="A115" t="s">
+        <v>330</v>
+      </c>
+      <c r="B115" t="s">
+        <v>335</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Updated data + code files.
</commit_message>
<xml_diff>
--- a/data/ecoli_interactions.xlsx
+++ b/data/ecoli_interactions.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\User\github\CARAMeL\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0EABC39C-85F1-4AAD-BCB4-1206B7252454}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{877DF00D-B4FE-4645-AE41-31925CBC8E48}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="22932" yWindow="-84" windowWidth="10080" windowHeight="17496" activeTab="1" xr2:uid="{ACD11B47-A1BF-4BB5-A276-4A778C038C67}"/>
+    <workbookView xWindow="22932" yWindow="-84" windowWidth="10080" windowHeight="17496" firstSheet="1" activeTab="1" xr2:uid="{ACD11B47-A1BF-4BB5-A276-4A778C038C67}"/>
   </bookViews>
   <sheets>
     <sheet name="identifiers" sheetId="10" r:id="rId1"/>
@@ -20,6 +20,7 @@
     <sheet name="MAGENTA_media" sheetId="4" r:id="rId5"/>
     <sheet name="Biolog" sheetId="8" r:id="rId6"/>
     <sheet name="Sequential" sheetId="9" r:id="rId7"/>
+    <sheet name="Russ_2018" sheetId="12" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -62,7 +63,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5172" uniqueCount="326">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="5317" uniqueCount="332">
   <si>
     <t>Code</t>
   </si>
@@ -1041,12 +1042,30 @@
   <si>
     <t>CEFSULODIN-6.0,MECILLINAM-0.03</t>
   </si>
+  <si>
+    <t>Drug_4</t>
+  </si>
+  <si>
+    <t>Drug_5</t>
+  </si>
+  <si>
+    <t>Drug_6</t>
+  </si>
+  <si>
+    <t>Drug_7</t>
+  </si>
+  <si>
+    <t>Drug_8</t>
+  </si>
+  <si>
+    <t>Drug_9</t>
+  </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="8" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -1082,6 +1101,27 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="12"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
   <fills count="2">
     <fill>
@@ -1100,11 +1140,12 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="1" applyFont="1"/>
@@ -1114,10 +1155,13 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" quotePrefix="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="2"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyFont="1"/>
   </cellXfs>
-  <cellStyles count="2">
+  <cellStyles count="3">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
     <cellStyle name="Normal 2" xfId="1" xr:uid="{3FA1BD6E-F028-44F2-8E24-C231F01CC9C4}"/>
+    <cellStyle name="Normal 3" xfId="2" xr:uid="{06CBA367-5EE8-4991-9A77-BCA541A117E3}"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -1726,7 +1770,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A80" sqref="A80:XFD80"/>
+      <selection pane="bottomLeft" activeCell="B98" sqref="B98"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -35794,4 +35838,1012 @@
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" horizontalDpi="1200" verticalDpi="1200" r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{12422BF5-5A3A-4AEC-BAC2-01333ECB181D}">
+  <dimension ref="A1:J50"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="12.44140625" defaultRowHeight="15.6" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="1" max="9" width="7" style="9" bestFit="1" customWidth="1"/>
+    <col min="10" max="10" width="12.6640625" style="9" bestFit="1" customWidth="1"/>
+    <col min="11" max="16384" width="12.44140625" style="9"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:10" s="10" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="1" t="s">
+        <v>36</v>
+      </c>
+      <c r="B1" s="1" t="s">
+        <v>37</v>
+      </c>
+      <c r="C1" s="1" t="s">
+        <v>51</v>
+      </c>
+      <c r="D1" s="1" t="s">
+        <v>326</v>
+      </c>
+      <c r="E1" s="1" t="s">
+        <v>327</v>
+      </c>
+      <c r="F1" s="1" t="s">
+        <v>328</v>
+      </c>
+      <c r="G1" s="1" t="s">
+        <v>329</v>
+      </c>
+      <c r="H1" s="1" t="s">
+        <v>330</v>
+      </c>
+      <c r="I1" s="1" t="s">
+        <v>331</v>
+      </c>
+      <c r="J1" s="1" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A2" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" t="s">
+        <v>28</v>
+      </c>
+      <c r="C2"/>
+      <c r="D2"/>
+      <c r="E2"/>
+      <c r="F2"/>
+      <c r="G2"/>
+      <c r="H2"/>
+      <c r="I2"/>
+      <c r="J2">
+        <v>-0.1871643401507678</v>
+      </c>
+    </row>
+    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A3" t="s">
+        <v>26</v>
+      </c>
+      <c r="B3" t="s">
+        <v>6</v>
+      </c>
+      <c r="C3"/>
+      <c r="D3"/>
+      <c r="E3"/>
+      <c r="F3"/>
+      <c r="G3"/>
+      <c r="H3"/>
+      <c r="I3"/>
+      <c r="J3">
+        <v>0.34221677398335204</v>
+      </c>
+    </row>
+    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C4"/>
+      <c r="D4"/>
+      <c r="E4"/>
+      <c r="F4"/>
+      <c r="G4"/>
+      <c r="H4"/>
+      <c r="I4"/>
+      <c r="J4">
+        <v>-0.24172993978671933</v>
+      </c>
+    </row>
+    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A5" t="s">
+        <v>26</v>
+      </c>
+      <c r="B5" t="s">
+        <v>7</v>
+      </c>
+      <c r="C5"/>
+      <c r="D5"/>
+      <c r="E5"/>
+      <c r="F5"/>
+      <c r="G5"/>
+      <c r="H5"/>
+      <c r="I5"/>
+      <c r="J5">
+        <v>0.49722644899362933</v>
+      </c>
+    </row>
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A6" t="s">
+        <v>26</v>
+      </c>
+      <c r="B6" t="s">
+        <v>4</v>
+      </c>
+      <c r="C6"/>
+      <c r="D6"/>
+      <c r="E6"/>
+      <c r="F6"/>
+      <c r="G6"/>
+      <c r="H6"/>
+      <c r="I6"/>
+      <c r="J6">
+        <v>0.78414687192478294</v>
+      </c>
+    </row>
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" t="s">
+        <v>26</v>
+      </c>
+      <c r="B7" t="s">
+        <v>304</v>
+      </c>
+      <c r="C7"/>
+      <c r="D7"/>
+      <c r="E7"/>
+      <c r="F7"/>
+      <c r="G7"/>
+      <c r="H7"/>
+      <c r="I7"/>
+      <c r="J7">
+        <v>1.0567276352914263</v>
+      </c>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" t="s">
+        <v>26</v>
+      </c>
+      <c r="B8" t="s">
+        <v>171</v>
+      </c>
+      <c r="C8"/>
+      <c r="D8"/>
+      <c r="E8"/>
+      <c r="F8"/>
+      <c r="G8"/>
+      <c r="H8"/>
+      <c r="I8"/>
+      <c r="J8">
+        <v>0.31443128336281423</v>
+      </c>
+    </row>
+    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A9" t="s">
+        <v>26</v>
+      </c>
+      <c r="B9" t="s">
+        <v>287</v>
+      </c>
+      <c r="C9"/>
+      <c r="D9"/>
+      <c r="E9"/>
+      <c r="F9"/>
+      <c r="G9"/>
+      <c r="H9"/>
+      <c r="I9"/>
+      <c r="J9">
+        <v>1.0443840797100683</v>
+      </c>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" t="s">
+        <v>28</v>
+      </c>
+      <c r="B10" t="s">
+        <v>6</v>
+      </c>
+      <c r="C10"/>
+      <c r="D10"/>
+      <c r="E10"/>
+      <c r="F10"/>
+      <c r="G10"/>
+      <c r="H10"/>
+      <c r="I10"/>
+      <c r="J10">
+        <v>0.17352711639641497</v>
+      </c>
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A11" t="s">
+        <v>28</v>
+      </c>
+      <c r="B11" t="s">
+        <v>10</v>
+      </c>
+      <c r="C11"/>
+      <c r="D11"/>
+      <c r="E11"/>
+      <c r="F11"/>
+      <c r="G11"/>
+      <c r="H11"/>
+      <c r="I11"/>
+      <c r="J11">
+        <v>-0.39730321495948934</v>
+      </c>
+    </row>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" t="s">
+        <v>7</v>
+      </c>
+      <c r="C12"/>
+      <c r="D12"/>
+      <c r="E12"/>
+      <c r="F12"/>
+      <c r="G12"/>
+      <c r="H12"/>
+      <c r="I12"/>
+      <c r="J12">
+        <v>0.7520101627037532</v>
+      </c>
+    </row>
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A13" t="s">
+        <v>28</v>
+      </c>
+      <c r="B13" t="s">
+        <v>4</v>
+      </c>
+      <c r="C13"/>
+      <c r="D13"/>
+      <c r="E13"/>
+      <c r="F13"/>
+      <c r="G13"/>
+      <c r="H13"/>
+      <c r="I13"/>
+      <c r="J13">
+        <v>0.96694814035037702</v>
+      </c>
+    </row>
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A14" t="s">
+        <v>28</v>
+      </c>
+      <c r="B14" t="s">
+        <v>304</v>
+      </c>
+      <c r="C14"/>
+      <c r="D14"/>
+      <c r="E14"/>
+      <c r="F14"/>
+      <c r="G14"/>
+      <c r="H14"/>
+      <c r="I14"/>
+      <c r="J14">
+        <v>1.4405263407632798</v>
+      </c>
+    </row>
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" t="s">
+        <v>171</v>
+      </c>
+      <c r="C15"/>
+      <c r="D15"/>
+      <c r="E15"/>
+      <c r="F15"/>
+      <c r="G15"/>
+      <c r="H15"/>
+      <c r="I15"/>
+      <c r="J15">
+        <v>0.84968428440383048</v>
+      </c>
+    </row>
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A16" t="s">
+        <v>28</v>
+      </c>
+      <c r="B16" t="s">
+        <v>287</v>
+      </c>
+      <c r="C16"/>
+      <c r="D16"/>
+      <c r="E16"/>
+      <c r="F16"/>
+      <c r="G16"/>
+      <c r="H16"/>
+      <c r="I16"/>
+      <c r="J16">
+        <v>0.51242663392905674</v>
+      </c>
+    </row>
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A17" t="s">
+        <v>6</v>
+      </c>
+      <c r="B17" t="s">
+        <v>10</v>
+      </c>
+      <c r="C17"/>
+      <c r="D17"/>
+      <c r="E17"/>
+      <c r="F17"/>
+      <c r="G17"/>
+      <c r="H17"/>
+      <c r="I17"/>
+      <c r="J17">
+        <v>0.10359300802984719</v>
+      </c>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A18" t="s">
+        <v>6</v>
+      </c>
+      <c r="B18" t="s">
+        <v>7</v>
+      </c>
+      <c r="C18"/>
+      <c r="D18"/>
+      <c r="E18"/>
+      <c r="F18"/>
+      <c r="G18"/>
+      <c r="H18"/>
+      <c r="I18"/>
+      <c r="J18">
+        <v>0.85246477718730362</v>
+      </c>
+    </row>
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A19" t="s">
+        <v>6</v>
+      </c>
+      <c r="B19" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19"/>
+      <c r="D19"/>
+      <c r="E19"/>
+      <c r="F19"/>
+      <c r="G19"/>
+      <c r="H19"/>
+      <c r="I19"/>
+      <c r="J19">
+        <v>1.3195706313367075</v>
+      </c>
+    </row>
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A20" t="s">
+        <v>6</v>
+      </c>
+      <c r="B20" t="s">
+        <v>304</v>
+      </c>
+      <c r="C20"/>
+      <c r="D20"/>
+      <c r="E20"/>
+      <c r="F20"/>
+      <c r="G20"/>
+      <c r="H20"/>
+      <c r="I20"/>
+      <c r="J20">
+        <v>0.82632197514755923</v>
+      </c>
+    </row>
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A21" t="s">
+        <v>6</v>
+      </c>
+      <c r="B21" t="s">
+        <v>171</v>
+      </c>
+      <c r="C21"/>
+      <c r="D21"/>
+      <c r="E21"/>
+      <c r="F21"/>
+      <c r="G21"/>
+      <c r="H21"/>
+      <c r="I21"/>
+      <c r="J21">
+        <v>0.27231189633613606</v>
+      </c>
+    </row>
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A22" t="s">
+        <v>6</v>
+      </c>
+      <c r="B22" t="s">
+        <v>287</v>
+      </c>
+      <c r="C22"/>
+      <c r="D22"/>
+      <c r="E22"/>
+      <c r="F22"/>
+      <c r="G22"/>
+      <c r="H22"/>
+      <c r="I22"/>
+      <c r="J22">
+        <v>0.57070703928778066</v>
+      </c>
+    </row>
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A23" t="s">
+        <v>10</v>
+      </c>
+      <c r="B23" t="s">
+        <v>7</v>
+      </c>
+      <c r="C23"/>
+      <c r="D23"/>
+      <c r="E23"/>
+      <c r="F23"/>
+      <c r="G23"/>
+      <c r="H23"/>
+      <c r="I23"/>
+      <c r="J23">
+        <v>0.57519192606738934</v>
+      </c>
+    </row>
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A24" t="s">
+        <v>10</v>
+      </c>
+      <c r="B24" t="s">
+        <v>4</v>
+      </c>
+      <c r="C24"/>
+      <c r="D24"/>
+      <c r="E24"/>
+      <c r="F24"/>
+      <c r="G24"/>
+      <c r="H24"/>
+      <c r="I24"/>
+      <c r="J24">
+        <v>0.9075103933687485</v>
+      </c>
+    </row>
+    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A25" t="s">
+        <v>10</v>
+      </c>
+      <c r="B25" t="s">
+        <v>304</v>
+      </c>
+      <c r="C25"/>
+      <c r="D25"/>
+      <c r="E25"/>
+      <c r="F25"/>
+      <c r="G25"/>
+      <c r="H25"/>
+      <c r="I25"/>
+      <c r="J25">
+        <v>0.44661768891756343</v>
+      </c>
+    </row>
+    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A26" t="s">
+        <v>10</v>
+      </c>
+      <c r="B26" t="s">
+        <v>171</v>
+      </c>
+      <c r="C26"/>
+      <c r="D26"/>
+      <c r="E26"/>
+      <c r="F26"/>
+      <c r="G26"/>
+      <c r="H26"/>
+      <c r="I26"/>
+      <c r="J26">
+        <v>-0.46792357990991046</v>
+      </c>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" t="s">
+        <v>10</v>
+      </c>
+      <c r="B27" t="s">
+        <v>287</v>
+      </c>
+      <c r="C27"/>
+      <c r="D27"/>
+      <c r="E27"/>
+      <c r="F27"/>
+      <c r="G27"/>
+      <c r="H27"/>
+      <c r="I27"/>
+      <c r="J27">
+        <v>0.44495690875396782</v>
+      </c>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" t="s">
+        <v>7</v>
+      </c>
+      <c r="B28" t="s">
+        <v>4</v>
+      </c>
+      <c r="C28"/>
+      <c r="D28"/>
+      <c r="E28"/>
+      <c r="F28"/>
+      <c r="G28"/>
+      <c r="H28"/>
+      <c r="I28"/>
+      <c r="J28">
+        <v>0.30815076703714595</v>
+      </c>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" t="s">
+        <v>7</v>
+      </c>
+      <c r="B29" t="s">
+        <v>304</v>
+      </c>
+      <c r="C29"/>
+      <c r="D29"/>
+      <c r="E29"/>
+      <c r="F29"/>
+      <c r="G29"/>
+      <c r="H29"/>
+      <c r="I29"/>
+      <c r="J29">
+        <v>0.51348098996300784</v>
+      </c>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" t="s">
+        <v>7</v>
+      </c>
+      <c r="B30" t="s">
+        <v>171</v>
+      </c>
+      <c r="C30"/>
+      <c r="D30"/>
+      <c r="E30"/>
+      <c r="F30"/>
+      <c r="G30"/>
+      <c r="H30"/>
+      <c r="I30"/>
+      <c r="J30">
+        <v>0.43319641821194377</v>
+      </c>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" t="s">
+        <v>7</v>
+      </c>
+      <c r="B31" t="s">
+        <v>287</v>
+      </c>
+      <c r="C31"/>
+      <c r="D31"/>
+      <c r="E31"/>
+      <c r="F31"/>
+      <c r="G31"/>
+      <c r="H31"/>
+      <c r="I31"/>
+      <c r="J31">
+        <v>-0.1085221380819313</v>
+      </c>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" t="s">
+        <v>4</v>
+      </c>
+      <c r="B32" t="s">
+        <v>304</v>
+      </c>
+      <c r="C32"/>
+      <c r="D32"/>
+      <c r="E32"/>
+      <c r="F32"/>
+      <c r="G32"/>
+      <c r="H32"/>
+      <c r="I32"/>
+      <c r="J32">
+        <v>0.77068571749455594</v>
+      </c>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" t="s">
+        <v>4</v>
+      </c>
+      <c r="B33" t="s">
+        <v>171</v>
+      </c>
+      <c r="C33"/>
+      <c r="D33"/>
+      <c r="E33"/>
+      <c r="F33"/>
+      <c r="G33"/>
+      <c r="H33"/>
+      <c r="I33"/>
+      <c r="J33">
+        <v>-8.3234772645520663E-2</v>
+      </c>
+    </row>
+    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A34" t="s">
+        <v>4</v>
+      </c>
+      <c r="B34" t="s">
+        <v>287</v>
+      </c>
+      <c r="C34"/>
+      <c r="D34"/>
+      <c r="E34"/>
+      <c r="F34"/>
+      <c r="G34"/>
+      <c r="H34"/>
+      <c r="I34"/>
+      <c r="J34">
+        <v>0.21640768126917501</v>
+      </c>
+    </row>
+    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A35" t="s">
+        <v>304</v>
+      </c>
+      <c r="B35" t="s">
+        <v>171</v>
+      </c>
+      <c r="C35"/>
+      <c r="D35"/>
+      <c r="E35"/>
+      <c r="F35"/>
+      <c r="G35"/>
+      <c r="H35"/>
+      <c r="I35"/>
+      <c r="J35">
+        <v>-1.4914424600200147</v>
+      </c>
+    </row>
+    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A36" t="s">
+        <v>304</v>
+      </c>
+      <c r="B36" t="s">
+        <v>287</v>
+      </c>
+      <c r="C36"/>
+      <c r="D36"/>
+      <c r="E36"/>
+      <c r="F36"/>
+      <c r="G36"/>
+      <c r="H36"/>
+      <c r="I36"/>
+      <c r="J36">
+        <v>0.18958536377063903</v>
+      </c>
+    </row>
+    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A37" t="s">
+        <v>171</v>
+      </c>
+      <c r="B37" t="s">
+        <v>287</v>
+      </c>
+      <c r="C37"/>
+      <c r="D37"/>
+      <c r="E37"/>
+      <c r="F37"/>
+      <c r="G37"/>
+      <c r="H37"/>
+      <c r="I37"/>
+      <c r="J37">
+        <v>-1.758785954766617E-2</v>
+      </c>
+    </row>
+    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A38" t="s">
+        <v>26</v>
+      </c>
+      <c r="B38" t="s">
+        <v>10</v>
+      </c>
+      <c r="C38" t="s">
+        <v>287</v>
+      </c>
+      <c r="D38"/>
+      <c r="E38"/>
+      <c r="F38"/>
+      <c r="G38"/>
+      <c r="H38"/>
+      <c r="I38"/>
+      <c r="J38">
+        <v>0.87185536128434205</v>
+      </c>
+    </row>
+    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A39" t="s">
+        <v>26</v>
+      </c>
+      <c r="B39" t="s">
+        <v>4</v>
+      </c>
+      <c r="C39" t="s">
+        <v>171</v>
+      </c>
+      <c r="D39"/>
+      <c r="E39"/>
+      <c r="F39"/>
+      <c r="G39"/>
+      <c r="H39"/>
+      <c r="I39"/>
+      <c r="J39">
+        <v>0.79074332108962575</v>
+      </c>
+    </row>
+    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A40" t="s">
+        <v>28</v>
+      </c>
+      <c r="B40" t="s">
+        <v>6</v>
+      </c>
+      <c r="C40" t="s">
+        <v>4</v>
+      </c>
+      <c r="D40"/>
+      <c r="E40"/>
+      <c r="F40"/>
+      <c r="G40"/>
+      <c r="H40"/>
+      <c r="I40"/>
+      <c r="J40">
+        <v>0.93688297331364756</v>
+      </c>
+    </row>
+    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A41" t="s">
+        <v>28</v>
+      </c>
+      <c r="B41" t="s">
+        <v>10</v>
+      </c>
+      <c r="C41" t="s">
+        <v>7</v>
+      </c>
+      <c r="D41"/>
+      <c r="E41"/>
+      <c r="F41"/>
+      <c r="G41"/>
+      <c r="H41"/>
+      <c r="I41"/>
+      <c r="J41">
+        <v>0.35138405155864305</v>
+      </c>
+    </row>
+    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A42" t="s">
+        <v>28</v>
+      </c>
+      <c r="B42" t="s">
+        <v>10</v>
+      </c>
+      <c r="C42" t="s">
+        <v>304</v>
+      </c>
+      <c r="D42"/>
+      <c r="E42"/>
+      <c r="F42"/>
+      <c r="G42"/>
+      <c r="H42"/>
+      <c r="I42"/>
+      <c r="J42">
+        <v>0.49883907797532212</v>
+      </c>
+    </row>
+    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A43" t="s">
+        <v>7</v>
+      </c>
+      <c r="B43" t="s">
+        <v>304</v>
+      </c>
+      <c r="C43" t="s">
+        <v>287</v>
+      </c>
+      <c r="D43"/>
+      <c r="E43"/>
+      <c r="F43"/>
+      <c r="G43"/>
+      <c r="H43"/>
+      <c r="I43"/>
+      <c r="J43">
+        <v>0.28189901119105187</v>
+      </c>
+    </row>
+    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A44" t="s">
+        <v>26</v>
+      </c>
+      <c r="B44" t="s">
+        <v>28</v>
+      </c>
+      <c r="C44" t="s">
+        <v>4</v>
+      </c>
+      <c r="D44" t="s">
+        <v>304</v>
+      </c>
+      <c r="E44" t="s">
+        <v>171</v>
+      </c>
+      <c r="F44"/>
+      <c r="G44"/>
+      <c r="H44"/>
+      <c r="I44"/>
+      <c r="J44">
+        <v>0.92625759227073945</v>
+      </c>
+    </row>
+    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A45" t="s">
+        <v>26</v>
+      </c>
+      <c r="B45" t="s">
+        <v>10</v>
+      </c>
+      <c r="C45" t="s">
+        <v>304</v>
+      </c>
+      <c r="D45" t="s">
+        <v>171</v>
+      </c>
+      <c r="E45" t="s">
+        <v>287</v>
+      </c>
+      <c r="F45"/>
+      <c r="G45"/>
+      <c r="H45"/>
+      <c r="I45"/>
+      <c r="J45">
+        <v>0.98236244255445659</v>
+      </c>
+    </row>
+    <row r="46" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>6</v>
+      </c>
+      <c r="B46" t="s">
+        <v>10</v>
+      </c>
+      <c r="C46" t="s">
+        <v>7</v>
+      </c>
+      <c r="D46" t="s">
+        <v>4</v>
+      </c>
+      <c r="E46" t="s">
+        <v>171</v>
+      </c>
+      <c r="F46"/>
+      <c r="G46"/>
+      <c r="H46"/>
+      <c r="I46"/>
+      <c r="J46">
+        <v>1.5319347849824387</v>
+      </c>
+    </row>
+    <row r="47" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>26</v>
+      </c>
+      <c r="B47" t="s">
+        <v>28</v>
+      </c>
+      <c r="C47" t="s">
+        <v>6</v>
+      </c>
+      <c r="D47" t="s">
+        <v>10</v>
+      </c>
+      <c r="E47" t="s">
+        <v>7</v>
+      </c>
+      <c r="F47" t="s">
+        <v>4</v>
+      </c>
+      <c r="G47" t="s">
+        <v>304</v>
+      </c>
+      <c r="H47"/>
+      <c r="I47"/>
+      <c r="J47">
+        <v>1.0352087944574611</v>
+      </c>
+    </row>
+    <row r="48" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>26</v>
+      </c>
+      <c r="B48" t="s">
+        <v>28</v>
+      </c>
+      <c r="C48" t="s">
+        <v>6</v>
+      </c>
+      <c r="D48" t="s">
+        <v>10</v>
+      </c>
+      <c r="E48" t="s">
+        <v>7</v>
+      </c>
+      <c r="F48" t="s">
+        <v>304</v>
+      </c>
+      <c r="G48" t="s">
+        <v>171</v>
+      </c>
+      <c r="H48"/>
+      <c r="I48"/>
+      <c r="J48">
+        <v>0.58089548958712156</v>
+      </c>
+    </row>
+    <row r="49" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>26</v>
+      </c>
+      <c r="B49" t="s">
+        <v>28</v>
+      </c>
+      <c r="C49" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" t="s">
+        <v>10</v>
+      </c>
+      <c r="E49" t="s">
+        <v>304</v>
+      </c>
+      <c r="F49" t="s">
+        <v>171</v>
+      </c>
+      <c r="G49" t="s">
+        <v>287</v>
+      </c>
+      <c r="H49"/>
+      <c r="I49"/>
+      <c r="J49">
+        <v>0.92338269829180974</v>
+      </c>
+    </row>
+    <row r="50" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>26</v>
+      </c>
+      <c r="B50" t="s">
+        <v>28</v>
+      </c>
+      <c r="C50" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" t="s">
+        <v>10</v>
+      </c>
+      <c r="E50" t="s">
+        <v>7</v>
+      </c>
+      <c r="F50" t="s">
+        <v>4</v>
+      </c>
+      <c r="G50" t="s">
+        <v>304</v>
+      </c>
+      <c r="H50" t="s">
+        <v>171</v>
+      </c>
+      <c r="I50" t="s">
+        <v>287</v>
+      </c>
+      <c r="J50">
+        <v>1.377649497652941</v>
+      </c>
+    </row>
+  </sheetData>
+  <phoneticPr fontId="6" type="noConversion"/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="4294967293" verticalDpi="0" r:id="rId1"/>
+</worksheet>
 </file>
</xml_diff>